<commit_message>
hoàn thiện import export kpi item
</commit_message>
<xml_diff>
--- a/DMS/Templates/Kpi_Item.xlsx
+++ b/DMS/Templates/Kpi_Item.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tai lieu du an\Rang Dong\DMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AFDAB71-3101-4DCB-B8D4-23DCAF10D348}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11430"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KPI nhân viên" sheetId="1" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>Năm</t>
   </si>
@@ -43,9 +44,6 @@
     <t>Tên nhân viên</t>
   </si>
   <si>
-    <t>{Mã NV- Tên nhân viên}</t>
-  </si>
-  <si>
     <t>{Mã NV}</t>
   </si>
   <si>
@@ -55,9 +53,6 @@
     <t>Sản lượng</t>
   </si>
   <si>
-    <t>Doanh số</t>
-  </si>
-  <si>
     <t>Số đơn hàng</t>
   </si>
   <si>
@@ -71,9 +66,6 @@
   </si>
   <si>
     <t>Tên sản phẩm</t>
-  </si>
-  <si>
-    <t>END - Vui lòng insert các mã sản phẩm vào theo từng nhân viên</t>
   </si>
   <si>
     <r>
@@ -114,11 +106,20 @@
 + Kết thúc ở dòng END</t>
     </r>
   </si>
+  <si>
+    <t>Doanh thu</t>
+  </si>
+  <si>
+    <t>Vui lòng insert các mã sản phẩm vào theo từng nhân viên</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -520,14 +521,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -540,7 +541,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C1" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
@@ -548,8 +549,8 @@
       <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
-        <v>12</v>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="2" t="s">
@@ -565,26 +566,28 @@
         <v>3</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="G4" s="10" t="s">
         <v>8</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -593,7 +596,7 @@
     </row>
     <row r="6" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -606,7 +609,7 @@
     </row>
     <row r="7" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -619,7 +622,7 @@
     </row>
     <row r="8" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
@@ -632,7 +635,7 @@
     </row>
     <row r="9" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -645,19 +648,22 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:C4"/>
+  <autoFilter ref="A4:C4" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="C1:F1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"2020,2021,2022,2023,2024,2025,2026,2027,2028,2029,2030"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Tháng 1, Tháng 2, Tháng 3, Tháng 4, Tháng 5, Tháng 6, Tháng 7, Tháng 8, Tháng 9, Tháng 10, Tháng 11, Tháng 12, Quý 1, Quý 2, Quý 3, Quý 4, Năm"</formula1>
     </dataValidation>
   </dataValidations>
@@ -666,7 +672,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>'San pham'!$B$2:$B$20</xm:f>
           </x14:formula1>
@@ -679,7 +685,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -694,10 +700,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -794,7 +800,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -808,7 +814,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="366.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>